<commit_message>
pretty the Table 1s
</commit_message>
<xml_diff>
--- a/documentation/Categorical_Tbl 1_with tests 2014.xlsx
+++ b/documentation/Categorical_Tbl 1_with tests 2014.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RProjects\github\BRFSS\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20756F80-C6F3-4B25-A5BB-C763388EB503}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC084B41-DBB4-4A33-A91D-16A4D4B03A59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-11820" yWindow="-14475" windowWidth="23340" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="82">
   <si>
     <t>Category</t>
   </si>
@@ -285,7 +285,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -327,6 +327,21 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -462,7 +477,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -484,9 +499,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -518,38 +530,47 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -909,71 +930,71 @@
     <col min="5" max="5" width="13" style="2" customWidth="1"/>
     <col min="6" max="6" width="13.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="1.7109375" style="1" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="0" style="11" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" style="12" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="0" style="13" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="10.28515625" style="12" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="0" style="13" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="0" style="10" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" style="11" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="0" style="12" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="10.28515625" style="11" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="0" style="12" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="10.28515625" style="5" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="1.7109375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="1.7109375" style="1" hidden="1" customWidth="1"/>
     <col min="15" max="16" width="0" style="1" hidden="1" customWidth="1"/>
     <col min="17" max="17" width="12.85546875" style="1" hidden="1" customWidth="1"/>
     <col min="18" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+      <c r="A1" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="29"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="19"/>
     </row>
     <row r="2" spans="1:17" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="G2" s="14"/>
-      <c r="H2" s="16" t="s">
+      <c r="G2" s="13"/>
+      <c r="H2" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="I2" s="17" t="s">
+      <c r="I2" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="J2" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="K2" s="17" t="s">
+      <c r="K2" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="L2" s="14" t="s">
+      <c r="L2" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="M2" s="17" t="s">
+      <c r="M2" s="16" t="s">
         <v>68</v>
       </c>
       <c r="O2" s="3" t="s">
@@ -987,43 +1008,43 @@
       </c>
     </row>
     <row r="3" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
-      <c r="B3" s="19" t="s">
+      <c r="A3" s="20"/>
+      <c r="B3" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="str">
+      <c r="C3" s="21" t="str">
         <f>H3 &amp; ", " &amp; ROUND((I3*100), 0) &amp; "%"</f>
         <v>58131, 100%</v>
       </c>
-      <c r="D3" s="2" t="str">
+      <c r="D3" s="21" t="str">
         <f>J3 &amp; ", " &amp; ROUND((K3*100), 0) &amp; "%"</f>
         <v>5343, 9%</v>
       </c>
-      <c r="E3" s="2" t="str">
+      <c r="E3" s="21" t="str">
         <f>L3 &amp; ", " &amp; ROUND((M3*100), 0) &amp; "%"</f>
         <v>52788, 91%</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="H3" s="11">
+      <c r="H3" s="10">
         <v>58131</v>
       </c>
-      <c r="I3" s="12">
+      <c r="I3" s="11">
         <f>H3/$O$3</f>
         <v>1</v>
       </c>
-      <c r="J3" s="11">
+      <c r="J3" s="10">
         <v>5343</v>
       </c>
-      <c r="K3" s="12">
+      <c r="K3" s="11">
         <f>J3/O3</f>
         <v>9.1913092842029212E-2</v>
       </c>
-      <c r="L3" s="11">
+      <c r="L3" s="10">
         <v>52788</v>
       </c>
-      <c r="M3" s="12">
+      <c r="M3" s="11">
         <f>L3/O3</f>
         <v>0.9080869071579708</v>
       </c>
@@ -1038,505 +1059,505 @@
       </c>
     </row>
     <row r="4" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="8" t="str">
+      <c r="C4" s="23" t="str">
         <f t="shared" ref="C4:C62" si="0">H4 &amp; ", " &amp; ROUND((I4*100), 0) &amp; "%"</f>
         <v>26169, 45%</v>
       </c>
-      <c r="D4" s="8" t="str">
+      <c r="D4" s="23" t="str">
         <f t="shared" ref="D4:D62" si="1">J4 &amp; ", " &amp; ROUND((K4*100), 0) &amp; "%"</f>
         <v>2671, 50%</v>
       </c>
-      <c r="E4" s="8" t="str">
+      <c r="E4" s="23" t="str">
         <f t="shared" ref="E4:E62" si="2">L4 &amp; ", " &amp; ROUND((M4*100), 0) &amp; "%"</f>
         <v>23498, 45%</v>
       </c>
-      <c r="F4" s="22" t="s">
+      <c r="F4" s="24" t="s">
         <v>79</v>
       </c>
       <c r="G4" s="7"/>
-      <c r="H4" s="9">
+      <c r="H4" s="8">
         <v>26169</v>
       </c>
-      <c r="I4" s="10">
+      <c r="I4" s="9">
         <f t="shared" ref="I4:I62" si="3">H4/$O$3</f>
         <v>0.45017288537957373</v>
       </c>
-      <c r="J4" s="9">
+      <c r="J4" s="8">
         <v>2671</v>
       </c>
-      <c r="K4" s="10">
+      <c r="K4" s="9">
         <f t="shared" ref="K4:K62" si="4">J4/$P$3</f>
         <v>0.49990641961444882</v>
       </c>
-      <c r="L4" s="9">
+      <c r="L4" s="8">
         <v>23498</v>
       </c>
-      <c r="M4" s="10">
+      <c r="M4" s="9">
         <f t="shared" ref="M4:M62" si="5">L4/$Q$3</f>
         <v>0.44513904675304994</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
-      <c r="B5" s="18" t="s">
+      <c r="A5" s="17"/>
+      <c r="B5" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="8" t="str">
+      <c r="C5" s="23" t="str">
         <f t="shared" si="0"/>
         <v>22646, 39%</v>
       </c>
-      <c r="D5" s="8" t="str">
+      <c r="D5" s="23" t="str">
         <f t="shared" si="1"/>
         <v>1897, 36%</v>
       </c>
-      <c r="E5" s="8" t="str">
+      <c r="E5" s="23" t="str">
         <f t="shared" si="2"/>
         <v>20749, 39%</v>
       </c>
-      <c r="F5" s="23"/>
+      <c r="F5" s="25"/>
       <c r="G5" s="7"/>
-      <c r="H5" s="9">
+      <c r="H5" s="8">
         <v>22646</v>
       </c>
-      <c r="I5" s="10">
+      <c r="I5" s="9">
         <f t="shared" si="3"/>
         <v>0.38956838863945226</v>
       </c>
-      <c r="J5" s="9">
+      <c r="J5" s="8">
         <v>1897</v>
       </c>
-      <c r="K5" s="10">
+      <c r="K5" s="9">
         <f t="shared" si="4"/>
         <v>0.35504398278120908</v>
       </c>
-      <c r="L5" s="9">
+      <c r="L5" s="8">
         <v>20749</v>
       </c>
-      <c r="M5" s="10">
+      <c r="M5" s="9">
         <f t="shared" si="5"/>
         <v>0.39306281730696369</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
-      <c r="B6" s="18" t="s">
+      <c r="A6" s="17"/>
+      <c r="B6" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="8" t="str">
+      <c r="C6" s="23" t="str">
         <f t="shared" si="0"/>
         <v>9316, 16%</v>
       </c>
-      <c r="D6" s="8" t="str">
+      <c r="D6" s="23" t="str">
         <f t="shared" si="1"/>
         <v>775, 15%</v>
       </c>
-      <c r="E6" s="8" t="str">
+      <c r="E6" s="23" t="str">
         <f t="shared" si="2"/>
         <v>8541, 16%</v>
       </c>
-      <c r="F6" s="24"/>
+      <c r="F6" s="26"/>
       <c r="G6" s="7"/>
-      <c r="H6" s="9">
+      <c r="H6" s="8">
         <v>9316</v>
       </c>
-      <c r="I6" s="10">
+      <c r="I6" s="9">
         <f t="shared" si="3"/>
         <v>0.16025872598097402</v>
       </c>
-      <c r="J6" s="9">
+      <c r="J6" s="8">
         <v>775</v>
       </c>
-      <c r="K6" s="10">
+      <c r="K6" s="9">
         <f t="shared" si="4"/>
         <v>0.14504959760434213</v>
       </c>
-      <c r="L6" s="9">
+      <c r="L6" s="8">
         <v>8541</v>
       </c>
-      <c r="M6" s="10">
+      <c r="M6" s="9">
         <f t="shared" si="5"/>
         <v>0.16179813593998635</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="8" t="str">
+      <c r="C7" s="23" t="str">
         <f t="shared" si="0"/>
         <v>899, 2%</v>
       </c>
-      <c r="D7" s="8" t="str">
+      <c r="D7" s="23" t="str">
         <f t="shared" si="1"/>
         <v>90, 2%</v>
       </c>
-      <c r="E7" s="8" t="str">
+      <c r="E7" s="23" t="str">
         <f t="shared" si="2"/>
         <v>809, 2%</v>
       </c>
-      <c r="F7" s="22" t="s">
+      <c r="F7" s="24" t="s">
         <v>79</v>
       </c>
       <c r="G7" s="7"/>
-      <c r="H7" s="9">
+      <c r="H7" s="8">
         <v>899</v>
       </c>
-      <c r="I7" s="10">
+      <c r="I7" s="9">
         <f t="shared" si="3"/>
         <v>1.5465070272315976E-2</v>
       </c>
-      <c r="J7" s="9">
+      <c r="J7" s="8">
         <v>90</v>
       </c>
-      <c r="K7" s="10">
+      <c r="K7" s="9">
         <f t="shared" si="4"/>
         <v>1.6844469399213923E-2</v>
       </c>
-      <c r="L7" s="9">
+      <c r="L7" s="8">
         <v>809</v>
       </c>
-      <c r="M7" s="10">
+      <c r="M7" s="9">
         <f t="shared" si="5"/>
         <v>1.5325452754413882E-2</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
-      <c r="B8" s="18" t="s">
+      <c r="A8" s="17"/>
+      <c r="B8" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="8" t="str">
+      <c r="C8" s="23" t="str">
         <f t="shared" si="0"/>
         <v>2657, 5%</v>
       </c>
-      <c r="D8" s="8" t="str">
+      <c r="D8" s="23" t="str">
         <f t="shared" si="1"/>
         <v>264, 5%</v>
       </c>
-      <c r="E8" s="8" t="str">
+      <c r="E8" s="23" t="str">
         <f t="shared" si="2"/>
         <v>2393, 5%</v>
       </c>
-      <c r="F8" s="23"/>
+      <c r="F8" s="25"/>
       <c r="G8" s="7"/>
-      <c r="H8" s="9">
+      <c r="H8" s="8">
         <v>2657</v>
       </c>
-      <c r="I8" s="10">
+      <c r="I8" s="9">
         <f t="shared" si="3"/>
         <v>4.5707109803719184E-2</v>
       </c>
-      <c r="J8" s="9">
+      <c r="J8" s="8">
         <v>264</v>
       </c>
-      <c r="K8" s="10">
+      <c r="K8" s="9">
         <f t="shared" si="4"/>
         <v>4.9410443571027515E-2</v>
       </c>
-      <c r="L8" s="9">
+      <c r="L8" s="8">
         <v>2393</v>
       </c>
-      <c r="M8" s="10">
+      <c r="M8" s="9">
         <f t="shared" si="5"/>
         <v>4.5332272486171096E-2</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
-      <c r="B9" s="18" t="s">
+      <c r="A9" s="17"/>
+      <c r="B9" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="8" t="str">
+      <c r="C9" s="23" t="str">
         <f t="shared" si="0"/>
         <v>3589, 6%</v>
       </c>
-      <c r="D9" s="8" t="str">
+      <c r="D9" s="23" t="str">
         <f t="shared" si="1"/>
         <v>325, 6%</v>
       </c>
-      <c r="E9" s="8" t="str">
+      <c r="E9" s="23" t="str">
         <f t="shared" si="2"/>
         <v>3264, 6%</v>
       </c>
-      <c r="F9" s="23"/>
+      <c r="F9" s="25"/>
       <c r="G9" s="7"/>
-      <c r="H9" s="9">
+      <c r="H9" s="8">
         <v>3589</v>
       </c>
-      <c r="I9" s="10">
+      <c r="I9" s="9">
         <f t="shared" si="3"/>
         <v>6.1739863411948877E-2</v>
       </c>
-      <c r="J9" s="9">
+      <c r="J9" s="8">
         <v>325</v>
       </c>
-      <c r="K9" s="10">
+      <c r="K9" s="9">
         <f t="shared" si="4"/>
         <v>6.0827250608272508E-2</v>
       </c>
-      <c r="L9" s="9">
+      <c r="L9" s="8">
         <v>3264</v>
       </c>
-      <c r="M9" s="10">
+      <c r="M9" s="9">
         <f t="shared" si="5"/>
         <v>6.1832234598772448E-2</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
-      <c r="B10" s="18" t="s">
+      <c r="A10" s="17"/>
+      <c r="B10" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="8" t="str">
+      <c r="C10" s="23" t="str">
         <f t="shared" si="0"/>
         <v>6543, 11%</v>
       </c>
-      <c r="D10" s="8" t="str">
+      <c r="D10" s="23" t="str">
         <f t="shared" si="1"/>
         <v>637, 12%</v>
       </c>
-      <c r="E10" s="8" t="str">
+      <c r="E10" s="23" t="str">
         <f t="shared" si="2"/>
         <v>5906, 11%</v>
       </c>
-      <c r="F10" s="23"/>
+      <c r="F10" s="25"/>
       <c r="G10" s="7"/>
-      <c r="H10" s="9">
+      <c r="H10" s="8">
         <v>6543</v>
       </c>
-      <c r="I10" s="10">
+      <c r="I10" s="9">
         <f t="shared" si="3"/>
         <v>0.11255612323889147</v>
       </c>
-      <c r="J10" s="9">
+      <c r="J10" s="8">
         <v>637</v>
       </c>
-      <c r="K10" s="10">
+      <c r="K10" s="9">
         <f t="shared" si="4"/>
         <v>0.11922141119221411</v>
       </c>
-      <c r="L10" s="9">
+      <c r="L10" s="8">
         <v>5906</v>
       </c>
-      <c r="M10" s="10">
+      <c r="M10" s="9">
         <f t="shared" si="5"/>
         <v>0.11188148821701902</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
-      <c r="B11" s="18" t="s">
+      <c r="A11" s="17"/>
+      <c r="B11" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="8" t="str">
+      <c r="C11" s="23" t="str">
         <f t="shared" si="0"/>
         <v>10724, 18%</v>
       </c>
-      <c r="D11" s="8" t="str">
+      <c r="D11" s="23" t="str">
         <f t="shared" si="1"/>
         <v>1153, 22%</v>
       </c>
-      <c r="E11" s="8" t="str">
+      <c r="E11" s="23" t="str">
         <f t="shared" si="2"/>
         <v>9571, 18%</v>
       </c>
-      <c r="F11" s="23"/>
+      <c r="F11" s="25"/>
       <c r="G11" s="7"/>
-      <c r="H11" s="9">
+      <c r="H11" s="8">
         <v>10724</v>
       </c>
-      <c r="I11" s="10">
+      <c r="I11" s="9">
         <f t="shared" si="3"/>
         <v>0.18447988164662574</v>
       </c>
-      <c r="J11" s="9">
+      <c r="J11" s="8">
         <v>1153</v>
       </c>
-      <c r="K11" s="10">
+      <c r="K11" s="9">
         <f t="shared" si="4"/>
         <v>0.21579636908104061</v>
       </c>
-      <c r="L11" s="9">
+      <c r="L11" s="8">
         <v>9571</v>
       </c>
-      <c r="M11" s="10">
+      <c r="M11" s="9">
         <f t="shared" si="5"/>
         <v>0.18131014624535879</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
-      <c r="B12" s="18" t="s">
+      <c r="A12" s="17"/>
+      <c r="B12" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="8" t="str">
+      <c r="C12" s="23" t="str">
         <f t="shared" si="0"/>
         <v>33719, 58%</v>
       </c>
-      <c r="D12" s="8" t="str">
+      <c r="D12" s="23" t="str">
         <f t="shared" si="1"/>
         <v>2874, 54%</v>
       </c>
-      <c r="E12" s="8" t="str">
+      <c r="E12" s="23" t="str">
         <f t="shared" si="2"/>
         <v>30845, 58%</v>
       </c>
-      <c r="F12" s="24"/>
+      <c r="F12" s="26"/>
       <c r="G12" s="7"/>
-      <c r="H12" s="9">
+      <c r="H12" s="8">
         <v>33719</v>
       </c>
-      <c r="I12" s="10">
+      <c r="I12" s="9">
         <f t="shared" si="3"/>
         <v>0.58005195162649881</v>
       </c>
-      <c r="J12" s="9">
+      <c r="J12" s="8">
         <v>2874</v>
       </c>
-      <c r="K12" s="10">
+      <c r="K12" s="9">
         <f t="shared" si="4"/>
         <v>0.53790005614823133</v>
       </c>
-      <c r="L12" s="9">
+      <c r="L12" s="8">
         <v>30845</v>
       </c>
-      <c r="M12" s="10">
+      <c r="M12" s="9">
         <f t="shared" si="5"/>
         <v>0.58431840569826476</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="8" t="str">
+      <c r="C13" s="23" t="str">
         <f t="shared" si="0"/>
         <v>52971, 91%</v>
       </c>
-      <c r="D13" s="8" t="str">
+      <c r="D13" s="23" t="str">
         <f t="shared" si="1"/>
         <v>4555, 85%</v>
       </c>
-      <c r="E13" s="8" t="str">
+      <c r="E13" s="23" t="str">
         <f t="shared" si="2"/>
         <v>48416, 92%</v>
       </c>
-      <c r="F13" s="22" t="s">
+      <c r="F13" s="24" t="s">
         <v>79</v>
       </c>
       <c r="G13" s="7"/>
-      <c r="H13" s="9">
+      <c r="H13" s="8">
         <v>52971</v>
       </c>
-      <c r="I13" s="10">
+      <c r="I13" s="9">
         <f t="shared" si="3"/>
         <v>0.91123496929349224</v>
       </c>
-      <c r="J13" s="9">
+      <c r="J13" s="8">
         <v>4555</v>
       </c>
-      <c r="K13" s="10">
+      <c r="K13" s="9">
         <f t="shared" si="4"/>
         <v>0.852517312371327</v>
       </c>
-      <c r="L13" s="9">
+      <c r="L13" s="8">
         <v>48416</v>
       </c>
-      <c r="M13" s="10">
+      <c r="M13" s="9">
         <f t="shared" si="5"/>
         <v>0.91717814654845797</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
-      <c r="B14" s="18" t="s">
+      <c r="A14" s="17"/>
+      <c r="B14" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="8" t="str">
+      <c r="C14" s="23" t="str">
         <f t="shared" si="0"/>
         <v>5160, 9%</v>
       </c>
-      <c r="D14" s="8" t="str">
+      <c r="D14" s="23" t="str">
         <f t="shared" si="1"/>
         <v>788, 15%</v>
       </c>
-      <c r="E14" s="8" t="str">
+      <c r="E14" s="23" t="str">
         <f t="shared" si="2"/>
         <v>4372, 8%</v>
       </c>
-      <c r="F14" s="24"/>
+      <c r="F14" s="26"/>
       <c r="G14" s="7"/>
-      <c r="H14" s="9">
+      <c r="H14" s="8">
         <v>5160</v>
       </c>
-      <c r="I14" s="10">
+      <c r="I14" s="9">
         <f t="shared" si="3"/>
         <v>8.8765030706507722E-2</v>
       </c>
-      <c r="J14" s="9">
+      <c r="J14" s="8">
         <v>788</v>
       </c>
-      <c r="K14" s="10">
+      <c r="K14" s="9">
         <f t="shared" si="4"/>
         <v>0.14748268762867303</v>
       </c>
-      <c r="L14" s="9">
+      <c r="L14" s="8">
         <v>4372</v>
       </c>
-      <c r="M14" s="10">
+      <c r="M14" s="9">
         <f t="shared" si="5"/>
         <v>8.2821853451542013E-2</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="2" t="str">
+      <c r="C15" s="21" t="str">
         <f t="shared" si="0"/>
         <v>2262, 4%</v>
       </c>
-      <c r="D15" s="2" t="str">
+      <c r="D15" s="21" t="str">
         <f t="shared" si="1"/>
         <v>236, 4%</v>
       </c>
-      <c r="E15" s="2" t="str">
+      <c r="E15" s="21" t="str">
         <f t="shared" si="2"/>
         <v>2026, 4%</v>
       </c>
-      <c r="F15" s="25">
+      <c r="F15" s="27">
         <v>9.2969999999999997E-2</v>
       </c>
-      <c r="H15" s="11">
+      <c r="H15" s="10">
         <v>2262</v>
       </c>
-      <c r="I15" s="12">
+      <c r="I15" s="11">
         <f t="shared" si="3"/>
         <v>3.8912112298085361E-2</v>
       </c>
-      <c r="J15" s="11">
+      <c r="J15" s="10">
         <v>236</v>
       </c>
-      <c r="K15" s="12">
+      <c r="K15" s="11">
         <f t="shared" si="4"/>
         <v>4.4169941980160957E-2</v>
       </c>
-      <c r="L15" s="11">
+      <c r="L15" s="10">
         <v>2026</v>
       </c>
       <c r="M15" s="5">
@@ -1545,38 +1566,38 @@
       </c>
     </row>
     <row r="16" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="19"/>
-      <c r="B16" s="19" t="s">
+      <c r="A16" s="20"/>
+      <c r="B16" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="2" t="str">
+      <c r="C16" s="21" t="str">
         <f t="shared" si="0"/>
         <v>55262, 95%</v>
       </c>
-      <c r="D16" s="2" t="str">
+      <c r="D16" s="21" t="str">
         <f t="shared" si="1"/>
         <v>5056, 95%</v>
       </c>
-      <c r="E16" s="2" t="str">
+      <c r="E16" s="21" t="str">
         <f t="shared" si="2"/>
         <v>50206, 95%</v>
       </c>
-      <c r="F16" s="26"/>
-      <c r="H16" s="11">
+      <c r="F16" s="28"/>
+      <c r="H16" s="10">
         <v>55262</v>
       </c>
-      <c r="I16" s="12">
+      <c r="I16" s="11">
         <f t="shared" si="3"/>
         <v>0.95064595482616843</v>
       </c>
-      <c r="J16" s="11">
+      <c r="J16" s="10">
         <v>5056</v>
       </c>
-      <c r="K16" s="12">
+      <c r="K16" s="11">
         <f t="shared" si="4"/>
         <v>0.94628485869361778</v>
       </c>
-      <c r="L16" s="11">
+      <c r="L16" s="10">
         <v>50206</v>
       </c>
       <c r="M16" s="5">
@@ -1585,38 +1606,38 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="19"/>
-      <c r="B17" s="19" t="s">
+      <c r="A17" s="20"/>
+      <c r="B17" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="2" t="str">
+      <c r="C17" s="21" t="str">
         <f t="shared" ref="C17" si="6">H17 &amp; ", " &amp; ROUND((I17*100), 0) &amp; "%"</f>
         <v>607, 1%</v>
       </c>
-      <c r="D17" s="2" t="str">
+      <c r="D17" s="21" t="str">
         <f t="shared" ref="D17" si="7">J17 &amp; ", " &amp; ROUND((K17*100), 0) &amp; "%"</f>
         <v>51, 1%</v>
       </c>
-      <c r="E17" s="2" t="str">
+      <c r="E17" s="21" t="str">
         <f t="shared" ref="E17" si="8">L17 &amp; ", " &amp; ROUND((M17*100), 0) &amp; "%"</f>
         <v>556, 1%</v>
       </c>
-      <c r="F17" s="27"/>
-      <c r="H17" s="11">
+      <c r="F17" s="29"/>
+      <c r="H17" s="10">
         <v>607</v>
       </c>
-      <c r="I17" s="12">
+      <c r="I17" s="11">
         <f t="shared" ref="I17" si="9">H17/$O$3</f>
         <v>1.0441932875746159E-2</v>
       </c>
-      <c r="J17" s="11">
+      <c r="J17" s="10">
         <v>51</v>
       </c>
-      <c r="K17" s="12">
+      <c r="K17" s="11">
         <f t="shared" si="4"/>
         <v>9.5451993262212244E-3</v>
       </c>
-      <c r="L17" s="11">
+      <c r="L17" s="10">
         <v>556</v>
       </c>
       <c r="M17" s="5">
@@ -1625,1888 +1646,1895 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="8" t="str">
+      <c r="C18" s="23" t="str">
         <f t="shared" si="0"/>
         <v>49394, 85%</v>
       </c>
-      <c r="D18" s="8" t="str">
+      <c r="D18" s="23" t="str">
         <f t="shared" si="1"/>
         <v>4362, 82%</v>
       </c>
-      <c r="E18" s="8" t="str">
+      <c r="E18" s="23" t="str">
         <f t="shared" si="2"/>
         <v>45032, 85%</v>
       </c>
-      <c r="F18" s="22" t="s">
+      <c r="F18" s="24" t="s">
         <v>79</v>
       </c>
       <c r="G18" s="7"/>
-      <c r="H18" s="9">
+      <c r="H18" s="8">
         <v>49394</v>
       </c>
-      <c r="I18" s="10">
+      <c r="I18" s="9">
         <f t="shared" si="3"/>
         <v>0.84970153618551203</v>
       </c>
-      <c r="J18" s="9">
+      <c r="J18" s="8">
         <v>4362</v>
       </c>
-      <c r="K18" s="10">
+      <c r="K18" s="9">
         <f t="shared" si="4"/>
         <v>0.81639528354856827</v>
       </c>
-      <c r="L18" s="9">
+      <c r="L18" s="8">
         <v>45032</v>
       </c>
-      <c r="M18" s="10">
+      <c r="M18" s="9">
         <f t="shared" si="5"/>
         <v>0.85307266803061299</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="18"/>
-      <c r="B19" s="18" t="s">
+      <c r="A19" s="17"/>
+      <c r="B19" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="8" t="str">
+      <c r="C19" s="23" t="str">
         <f t="shared" si="0"/>
         <v>3939, 7%</v>
       </c>
-      <c r="D19" s="8" t="str">
+      <c r="D19" s="23" t="str">
         <f t="shared" si="1"/>
         <v>411, 8%</v>
       </c>
-      <c r="E19" s="8" t="str">
+      <c r="E19" s="23" t="str">
         <f t="shared" si="2"/>
         <v>3528, 7%</v>
       </c>
-      <c r="F19" s="23"/>
+      <c r="F19" s="25"/>
       <c r="G19" s="7"/>
-      <c r="H19" s="9">
+      <c r="H19" s="8">
         <v>3939</v>
       </c>
-      <c r="I19" s="10">
+      <c r="I19" s="9">
         <f t="shared" si="3"/>
         <v>6.7760747277700373E-2</v>
       </c>
-      <c r="J19" s="9">
+      <c r="J19" s="8">
         <v>411</v>
       </c>
-      <c r="K19" s="10">
+      <c r="K19" s="9">
         <f t="shared" si="4"/>
         <v>7.6923076923076927E-2</v>
       </c>
-      <c r="L19" s="9">
+      <c r="L19" s="8">
         <v>3528</v>
       </c>
-      <c r="M19" s="10">
+      <c r="M19" s="9">
         <f t="shared" si="5"/>
         <v>6.6833371220731991E-2</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="18"/>
-      <c r="B20" s="18" t="s">
+      <c r="A20" s="17"/>
+      <c r="B20" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="8" t="str">
+      <c r="C20" s="23" t="str">
         <f t="shared" si="0"/>
         <v>930, 2%</v>
       </c>
-      <c r="D20" s="8" t="str">
+      <c r="D20" s="23" t="str">
         <f t="shared" si="1"/>
         <v>153, 3%</v>
       </c>
-      <c r="E20" s="8" t="str">
+      <c r="E20" s="23" t="str">
         <f t="shared" si="2"/>
         <v>777, 1%</v>
       </c>
-      <c r="F20" s="23"/>
+      <c r="F20" s="25"/>
       <c r="G20" s="7"/>
-      <c r="H20" s="9">
+      <c r="H20" s="8">
         <v>930</v>
       </c>
-      <c r="I20" s="10">
+      <c r="I20" s="9">
         <f t="shared" si="3"/>
         <v>1.5998348557568251E-2</v>
       </c>
-      <c r="J20" s="9">
+      <c r="J20" s="8">
         <v>153</v>
       </c>
-      <c r="K20" s="10">
+      <c r="K20" s="9">
         <f t="shared" si="4"/>
         <v>2.8635597978663673E-2</v>
       </c>
-      <c r="L20" s="9">
+      <c r="L20" s="8">
         <v>777</v>
       </c>
-      <c r="M20" s="10">
+      <c r="M20" s="9">
         <f t="shared" si="5"/>
         <v>1.4719254375994544E-2</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="18"/>
-      <c r="B21" s="18" t="s">
+      <c r="A21" s="17"/>
+      <c r="B21" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="8" t="str">
+      <c r="C21" s="23" t="str">
         <f t="shared" si="0"/>
         <v>557, 1%</v>
       </c>
-      <c r="D21" s="8" t="str">
+      <c r="D21" s="23" t="str">
         <f t="shared" si="1"/>
         <v>51, 1%</v>
       </c>
-      <c r="E21" s="8" t="str">
+      <c r="E21" s="23" t="str">
         <f t="shared" si="2"/>
         <v>506, 1%</v>
       </c>
-      <c r="F21" s="23"/>
+      <c r="F21" s="25"/>
       <c r="G21" s="7"/>
-      <c r="H21" s="9">
+      <c r="H21" s="8">
         <v>557</v>
       </c>
-      <c r="I21" s="10">
+      <c r="I21" s="9">
         <f t="shared" si="3"/>
         <v>9.5818066092102326E-3</v>
       </c>
-      <c r="J21" s="9">
+      <c r="J21" s="8">
         <v>51</v>
       </c>
-      <c r="K21" s="10">
+      <c r="K21" s="9">
         <f t="shared" si="4"/>
         <v>9.5451993262212244E-3</v>
       </c>
-      <c r="L21" s="9">
+      <c r="L21" s="8">
         <v>506</v>
       </c>
-      <c r="M21" s="10">
+      <c r="M21" s="9">
         <f t="shared" si="5"/>
         <v>9.585511858755778E-3</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="18"/>
-      <c r="B22" s="18" t="s">
+      <c r="A22" s="17"/>
+      <c r="B22" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="C22" s="8" t="str">
+      <c r="C22" s="23" t="str">
         <f t="shared" ref="C22" si="10">H22 &amp; ", " &amp; ROUND((I22*100), 0) &amp; "%"</f>
         <v>261, 0%</v>
       </c>
-      <c r="D22" s="8" t="str">
+      <c r="D22" s="23" t="str">
         <f t="shared" ref="D22" si="11">J22 &amp; ", " &amp; ROUND((K22*100), 0) &amp; "%"</f>
         <v>20, 0%</v>
       </c>
-      <c r="E22" s="8" t="str">
+      <c r="E22" s="23" t="str">
         <f t="shared" ref="E22" si="12">L22 &amp; ", " &amp; ROUND((M22*100), 0) &amp; "%"</f>
         <v>241, 0%</v>
       </c>
-      <c r="F22" s="23"/>
+      <c r="F22" s="25"/>
       <c r="G22" s="7"/>
-      <c r="H22" s="9">
+      <c r="H22" s="8">
         <v>261</v>
       </c>
-      <c r="I22" s="10">
+      <c r="I22" s="9">
         <f t="shared" si="3"/>
         <v>4.4898591113175417E-3</v>
       </c>
-      <c r="J22" s="9">
+      <c r="J22" s="8">
         <v>20</v>
       </c>
-      <c r="K22" s="10">
+      <c r="K22" s="9">
         <f t="shared" si="4"/>
         <v>3.7432154220475387E-3</v>
       </c>
-      <c r="L22" s="9">
+      <c r="L22" s="8">
         <v>241</v>
       </c>
-      <c r="M22" s="10">
+      <c r="M22" s="9">
         <f t="shared" si="5"/>
         <v>4.5654315374706374E-3</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="18"/>
-      <c r="B23" s="18" t="s">
+      <c r="A23" s="17"/>
+      <c r="B23" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="8" t="str">
+      <c r="C23" s="23" t="str">
         <f t="shared" si="0"/>
         <v>2056, 4%</v>
       </c>
-      <c r="D23" s="8" t="str">
+      <c r="D23" s="23" t="str">
         <f t="shared" si="1"/>
         <v>252, 5%</v>
       </c>
-      <c r="E23" s="8" t="str">
+      <c r="E23" s="23" t="str">
         <f t="shared" si="2"/>
         <v>1804, 3%</v>
       </c>
-      <c r="F23" s="23"/>
+      <c r="F23" s="25"/>
       <c r="G23" s="7"/>
-      <c r="H23" s="9">
+      <c r="H23" s="8">
         <v>2056</v>
       </c>
-      <c r="I23" s="10">
+      <c r="I23" s="9">
         <f t="shared" si="3"/>
         <v>3.5368392079957338E-2</v>
       </c>
-      <c r="J23" s="9">
+      <c r="J23" s="8">
         <v>252</v>
       </c>
-      <c r="K23" s="10">
+      <c r="K23" s="9">
         <f t="shared" si="4"/>
         <v>4.7164514317798986E-2</v>
       </c>
-      <c r="L23" s="9">
+      <c r="L23" s="8">
         <v>1804</v>
       </c>
-      <c r="M23" s="10">
+      <c r="M23" s="9">
         <f t="shared" si="5"/>
         <v>3.4174433583390167E-2</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="18"/>
-      <c r="B24" s="18" t="s">
+      <c r="A24" s="17"/>
+      <c r="B24" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C24" s="8" t="str">
+      <c r="C24" s="23" t="str">
         <f t="shared" si="0"/>
         <v>994, 2%</v>
       </c>
-      <c r="D24" s="8" t="str">
+      <c r="D24" s="23" t="str">
         <f t="shared" si="1"/>
         <v>94, 2%</v>
       </c>
-      <c r="E24" s="8" t="str">
+      <c r="E24" s="23" t="str">
         <f t="shared" si="2"/>
         <v>900, 2%</v>
       </c>
-      <c r="F24" s="24"/>
+      <c r="F24" s="26"/>
       <c r="G24" s="7"/>
-      <c r="H24" s="9">
+      <c r="H24" s="8">
         <v>994</v>
       </c>
-      <c r="I24" s="10">
+      <c r="I24" s="9">
         <f t="shared" si="3"/>
         <v>1.7099310178734239E-2</v>
       </c>
-      <c r="J24" s="9">
+      <c r="J24" s="8">
         <v>94</v>
       </c>
-      <c r="K24" s="10">
+      <c r="K24" s="9">
         <f t="shared" si="4"/>
         <v>1.7593112483623434E-2</v>
       </c>
-      <c r="L24" s="9">
+      <c r="L24" s="8">
         <v>900</v>
       </c>
-      <c r="M24" s="10">
+      <c r="M24" s="9">
         <f t="shared" si="5"/>
         <v>1.7049329393043874E-2</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="18" t="s">
+      <c r="A25" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="B25" s="18" t="s">
+      <c r="B25" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="C25" s="8" t="str">
+      <c r="C25" s="23" t="str">
         <f t="shared" si="0"/>
         <v>40551, 70%</v>
       </c>
-      <c r="D25" s="8" t="str">
+      <c r="D25" s="23" t="str">
         <f t="shared" si="1"/>
         <v>3530, 66%</v>
       </c>
-      <c r="E25" s="8" t="str">
+      <c r="E25" s="23" t="str">
         <f t="shared" si="2"/>
         <v>37021, 70%</v>
       </c>
-      <c r="F25" s="22" t="s">
+      <c r="F25" s="24" t="s">
         <v>79</v>
       </c>
       <c r="G25" s="7"/>
-      <c r="H25" s="9">
+      <c r="H25" s="8">
         <v>40551</v>
       </c>
-      <c r="I25" s="10">
+      <c r="I25" s="9">
         <f t="shared" si="3"/>
         <v>0.69757960468596791</v>
       </c>
-      <c r="J25" s="9">
+      <c r="J25" s="8">
         <v>3530</v>
       </c>
-      <c r="K25" s="10">
+      <c r="K25" s="9">
         <f t="shared" si="4"/>
         <v>0.66067752199139063</v>
       </c>
-      <c r="L25" s="9">
+      <c r="L25" s="8">
         <v>37021</v>
       </c>
-      <c r="M25" s="10">
+      <c r="M25" s="9">
         <f t="shared" si="5"/>
         <v>0.70131469273319691</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="18"/>
-      <c r="B26" s="18" t="s">
+      <c r="A26" s="17"/>
+      <c r="B26" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="C26" s="8" t="str">
+      <c r="C26" s="23" t="str">
         <f t="shared" si="0"/>
         <v>15588, 27%</v>
       </c>
-      <c r="D26" s="8" t="str">
+      <c r="D26" s="23" t="str">
         <f t="shared" si="1"/>
         <v>1577, 30%</v>
       </c>
-      <c r="E26" s="8" t="str">
+      <c r="E26" s="23" t="str">
         <f t="shared" si="2"/>
         <v>14011, 27%</v>
       </c>
-      <c r="F26" s="23"/>
+      <c r="F26" s="25"/>
       <c r="G26" s="7"/>
-      <c r="H26" s="9">
+      <c r="H26" s="8">
         <v>15588</v>
       </c>
-      <c r="I26" s="10">
+      <c r="I26" s="9">
         <f t="shared" si="3"/>
         <v>0.26815296485524076</v>
       </c>
-      <c r="J26" s="9">
+      <c r="J26" s="8">
         <v>1577</v>
       </c>
-      <c r="K26" s="10">
+      <c r="K26" s="9">
         <f t="shared" si="4"/>
         <v>0.29515253602844843</v>
       </c>
-      <c r="L26" s="9">
+      <c r="L26" s="8">
         <v>14011</v>
       </c>
-      <c r="M26" s="10">
+      <c r="M26" s="9">
         <f t="shared" si="5"/>
         <v>0.26542017125104189</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="18"/>
-      <c r="B27" s="18" t="s">
+      <c r="A27" s="17"/>
+      <c r="B27" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C27" s="8" t="str">
+      <c r="C27" s="23" t="str">
         <f t="shared" si="0"/>
         <v>982, 2%</v>
       </c>
-      <c r="D27" s="8" t="str">
+      <c r="D27" s="23" t="str">
         <f t="shared" si="1"/>
         <v>134, 3%</v>
       </c>
-      <c r="E27" s="8" t="str">
+      <c r="E27" s="23" t="str">
         <f t="shared" si="2"/>
         <v>848, 2%</v>
       </c>
-      <c r="F27" s="23"/>
+      <c r="F27" s="25"/>
       <c r="G27" s="7"/>
-      <c r="H27" s="9">
+      <c r="H27" s="8">
         <v>982</v>
       </c>
-      <c r="I27" s="10">
+      <c r="I27" s="9">
         <f t="shared" si="3"/>
         <v>1.6892879874765617E-2</v>
       </c>
-      <c r="J27" s="9">
+      <c r="J27" s="8">
         <v>134</v>
       </c>
-      <c r="K27" s="10">
+      <c r="K27" s="9">
         <f t="shared" si="4"/>
         <v>2.5079543327718511E-2</v>
       </c>
-      <c r="L27" s="9">
+      <c r="L27" s="8">
         <v>848</v>
       </c>
-      <c r="M27" s="10">
+      <c r="M27" s="9">
         <f t="shared" si="5"/>
         <v>1.6064257028112448E-2</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="18"/>
-      <c r="B28" s="18" t="s">
+      <c r="A28" s="17"/>
+      <c r="B28" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C28" s="8" t="str">
+      <c r="C28" s="23" t="str">
         <f t="shared" si="0"/>
         <v>1010, 2%</v>
       </c>
-      <c r="D28" s="8" t="str">
+      <c r="D28" s="23" t="str">
         <f t="shared" si="1"/>
         <v>102, 2%</v>
       </c>
-      <c r="E28" s="8" t="str">
+      <c r="E28" s="23" t="str">
         <f t="shared" si="2"/>
         <v>908, 2%</v>
       </c>
-      <c r="F28" s="24"/>
+      <c r="F28" s="26"/>
       <c r="G28" s="7"/>
-      <c r="H28" s="9">
+      <c r="H28" s="8">
         <v>1010</v>
       </c>
-      <c r="I28" s="10">
+      <c r="I28" s="9">
         <f t="shared" si="3"/>
         <v>1.7374550584025737E-2</v>
       </c>
-      <c r="J28" s="9">
+      <c r="J28" s="8">
         <v>102</v>
       </c>
-      <c r="K28" s="10">
+      <c r="K28" s="9">
         <f t="shared" si="4"/>
         <v>1.9090398652442449E-2</v>
       </c>
-      <c r="L28" s="9">
+      <c r="L28" s="8">
         <v>908</v>
       </c>
-      <c r="M28" s="10">
+      <c r="M28" s="9">
         <f t="shared" si="5"/>
         <v>1.7200878987648709E-2</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="18" t="s">
+      <c r="A29" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="B29" s="18" t="s">
+      <c r="B29" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="C29" s="8" t="str">
+      <c r="C29" s="23" t="str">
         <f t="shared" si="0"/>
         <v>2483, 4%</v>
       </c>
-      <c r="D29" s="8" t="str">
+      <c r="D29" s="23" t="str">
         <f t="shared" si="1"/>
         <v>318, 6%</v>
       </c>
-      <c r="E29" s="8" t="str">
+      <c r="E29" s="23" t="str">
         <f t="shared" si="2"/>
         <v>2165, 4%</v>
       </c>
-      <c r="F29" s="22" t="s">
+      <c r="F29" s="24" t="s">
         <v>79</v>
       </c>
       <c r="G29" s="7"/>
-      <c r="H29" s="9">
+      <c r="H29" s="8">
         <v>2483</v>
       </c>
-      <c r="I29" s="10">
+      <c r="I29" s="9">
         <f t="shared" si="3"/>
         <v>4.2713870396174157E-2</v>
       </c>
-      <c r="J29" s="9">
+      <c r="J29" s="8">
         <v>318</v>
       </c>
-      <c r="K29" s="10">
+      <c r="K29" s="9">
         <f t="shared" si="4"/>
         <v>5.9517125210555868E-2</v>
       </c>
-      <c r="L29" s="9">
+      <c r="L29" s="8">
         <v>2165</v>
       </c>
-      <c r="M29" s="10">
+      <c r="M29" s="9">
         <f t="shared" si="5"/>
         <v>4.101310903993332E-2</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30" s="18"/>
-      <c r="B30" s="18" t="s">
+      <c r="A30" s="17"/>
+      <c r="B30" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="C30" s="8" t="str">
+      <c r="C30" s="23" t="str">
         <f t="shared" ref="C30" si="13">H30 &amp; ", " &amp; ROUND((I30*100), 0) &amp; "%"</f>
         <v>16241, 28%</v>
       </c>
-      <c r="D30" s="8" t="str">
+      <c r="D30" s="23" t="str">
         <f t="shared" ref="D30" si="14">J30 &amp; ", " &amp; ROUND((K30*100), 0) &amp; "%"</f>
         <v>1430, 27%</v>
       </c>
-      <c r="E30" s="8" t="str">
+      <c r="E30" s="23" t="str">
         <f t="shared" ref="E30" si="15">L30 &amp; ", " &amp; ROUND((M30*100), 0) &amp; "%"</f>
         <v>14811, 28%</v>
       </c>
-      <c r="F30" s="23"/>
+      <c r="F30" s="25"/>
       <c r="G30" s="7"/>
-      <c r="H30" s="9">
+      <c r="H30" s="8">
         <v>16241</v>
       </c>
-      <c r="I30" s="10">
+      <c r="I30" s="9">
         <f t="shared" si="3"/>
         <v>0.27938621389619994</v>
       </c>
-      <c r="J30" s="9">
+      <c r="J30" s="8">
         <v>1430</v>
       </c>
-      <c r="K30" s="10">
+      <c r="K30" s="9">
         <f t="shared" si="4"/>
         <v>0.26763990267639903</v>
       </c>
-      <c r="L30" s="9">
+      <c r="L30" s="8">
         <v>14811</v>
       </c>
-      <c r="M30" s="10">
+      <c r="M30" s="9">
         <f t="shared" si="5"/>
         <v>0.28057513071152534</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="18"/>
-      <c r="B31" s="18" t="s">
+      <c r="A31" s="17"/>
+      <c r="B31" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C31" s="8" t="str">
+      <c r="C31" s="23" t="str">
         <f t="shared" si="0"/>
         <v>17559, 30%</v>
       </c>
-      <c r="D31" s="8" t="str">
+      <c r="D31" s="23" t="str">
         <f t="shared" si="1"/>
         <v>1720, 32%</v>
       </c>
-      <c r="E31" s="8" t="str">
+      <c r="E31" s="23" t="str">
         <f t="shared" si="2"/>
         <v>15839, 30%</v>
       </c>
-      <c r="F31" s="23"/>
+      <c r="F31" s="25"/>
       <c r="G31" s="7"/>
-      <c r="H31" s="9">
+      <c r="H31" s="8">
         <v>17559</v>
       </c>
-      <c r="I31" s="10">
+      <c r="I31" s="9">
         <f t="shared" si="3"/>
         <v>0.30205914228208702</v>
       </c>
-      <c r="J31" s="9">
+      <c r="J31" s="8">
         <v>1720</v>
       </c>
-      <c r="K31" s="10">
+      <c r="K31" s="9">
         <f t="shared" si="4"/>
         <v>0.32191652629608836</v>
       </c>
-      <c r="L31" s="9">
+      <c r="L31" s="8">
         <v>15839</v>
       </c>
-      <c r="M31" s="10">
+      <c r="M31" s="9">
         <f t="shared" si="5"/>
         <v>0.30004925361824658</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A32" s="18"/>
-      <c r="B32" s="18" t="s">
+      <c r="A32" s="17"/>
+      <c r="B32" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="8" t="str">
+      <c r="C32" s="23" t="str">
         <f t="shared" si="0"/>
         <v>21742, 37%</v>
       </c>
-      <c r="D32" s="8" t="str">
+      <c r="D32" s="23" t="str">
         <f t="shared" si="1"/>
         <v>1868, 35%</v>
       </c>
-      <c r="E32" s="8" t="str">
+      <c r="E32" s="23" t="str">
         <f t="shared" si="2"/>
         <v>19874, 38%</v>
       </c>
-      <c r="F32" s="23"/>
+      <c r="F32" s="25"/>
       <c r="G32" s="7"/>
-      <c r="H32" s="9">
+      <c r="H32" s="8">
         <v>21742</v>
       </c>
-      <c r="I32" s="10">
+      <c r="I32" s="9">
         <f t="shared" si="3"/>
         <v>0.3740173057404827</v>
       </c>
-      <c r="J32" s="9">
+      <c r="J32" s="8">
         <v>1868</v>
       </c>
-      <c r="K32" s="10">
+      <c r="K32" s="9">
         <f t="shared" si="4"/>
         <v>0.34961632041924012</v>
       </c>
-      <c r="L32" s="9">
+      <c r="L32" s="8">
         <v>19874</v>
       </c>
-      <c r="M32" s="10">
+      <c r="M32" s="9">
         <f t="shared" si="5"/>
         <v>0.37648708039705991</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33" s="18"/>
-      <c r="B33" s="18" t="s">
+      <c r="A33" s="17"/>
+      <c r="B33" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C33" s="8" t="str">
+      <c r="C33" s="23" t="str">
         <f t="shared" si="0"/>
         <v>106, 0%</v>
       </c>
-      <c r="D33" s="8" t="str">
+      <c r="D33" s="23" t="str">
         <f t="shared" si="1"/>
         <v>7, 0%</v>
       </c>
-      <c r="E33" s="8" t="str">
+      <c r="E33" s="23" t="str">
         <f t="shared" si="2"/>
         <v>99, 0%</v>
       </c>
-      <c r="F33" s="24"/>
+      <c r="F33" s="26"/>
       <c r="G33" s="7"/>
-      <c r="H33" s="9">
+      <c r="H33" s="8">
         <v>106</v>
       </c>
-      <c r="I33" s="10">
+      <c r="I33" s="9">
         <f t="shared" si="3"/>
         <v>1.8234676850561661E-3</v>
       </c>
-      <c r="J33" s="9">
+      <c r="J33" s="8">
         <v>7</v>
       </c>
-      <c r="K33" s="10">
+      <c r="K33" s="9">
         <f t="shared" si="4"/>
         <v>1.3101253977166386E-3</v>
       </c>
-      <c r="L33" s="9">
+      <c r="L33" s="8">
         <v>99</v>
       </c>
-      <c r="M33" s="10">
+      <c r="M33" s="9">
         <f t="shared" si="5"/>
         <v>1.8754262332348261E-3</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="18" t="s">
+      <c r="A34" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="B34" s="18" t="s">
+      <c r="B34" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="C34" s="8" t="str">
+      <c r="C34" s="23" t="str">
         <f t="shared" si="0"/>
         <v>1165, 2%</v>
       </c>
-      <c r="D34" s="8" t="str">
+      <c r="D34" s="23" t="str">
         <f t="shared" si="1"/>
         <v>187, 3%</v>
       </c>
-      <c r="E34" s="8" t="str">
+      <c r="E34" s="23" t="str">
         <f t="shared" si="2"/>
         <v>978, 2%</v>
       </c>
-      <c r="F34" s="22" t="s">
+      <c r="F34" s="24" t="s">
         <v>79</v>
       </c>
       <c r="G34" s="7"/>
-      <c r="H34" s="9">
+      <c r="H34" s="8">
         <v>1165</v>
       </c>
-      <c r="I34" s="10">
+      <c r="I34" s="9">
         <f t="shared" si="3"/>
         <v>2.0040942010287111E-2</v>
       </c>
-      <c r="J34" s="9">
+      <c r="J34" s="8">
         <v>187</v>
       </c>
-      <c r="K34" s="10">
+      <c r="K34" s="9">
         <f t="shared" si="4"/>
         <v>3.4999064196144486E-2</v>
       </c>
-      <c r="L34" s="9">
+      <c r="L34" s="8">
         <v>978</v>
       </c>
-      <c r="M34" s="10">
+      <c r="M34" s="9">
         <f t="shared" si="5"/>
         <v>1.852693794044101E-2</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35" s="18"/>
-      <c r="B35" s="18" t="s">
+      <c r="A35" s="17"/>
+      <c r="B35" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="C35" s="8" t="str">
+      <c r="C35" s="23" t="str">
         <f t="shared" si="0"/>
         <v>2111, 4%</v>
       </c>
-      <c r="D35" s="8" t="str">
+      <c r="D35" s="23" t="str">
         <f t="shared" si="1"/>
         <v>305, 6%</v>
       </c>
-      <c r="E35" s="8" t="str">
+      <c r="E35" s="23" t="str">
         <f t="shared" si="2"/>
         <v>1806, 3%</v>
       </c>
-      <c r="F35" s="23"/>
+      <c r="F35" s="25"/>
       <c r="G35" s="7"/>
-      <c r="H35" s="9">
+      <c r="H35" s="8">
         <v>2111</v>
       </c>
-      <c r="I35" s="10">
+      <c r="I35" s="9">
         <f t="shared" si="3"/>
         <v>3.6314530973146859E-2</v>
       </c>
-      <c r="J35" s="9">
+      <c r="J35" s="8">
         <v>305</v>
       </c>
-      <c r="K35" s="10">
+      <c r="K35" s="9">
         <f t="shared" si="4"/>
         <v>5.7084035186224964E-2</v>
       </c>
-      <c r="L35" s="9">
+      <c r="L35" s="8">
         <v>1806</v>
       </c>
-      <c r="M35" s="10">
+      <c r="M35" s="9">
         <f t="shared" si="5"/>
         <v>3.4212320982041376E-2</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A36" s="18"/>
-      <c r="B36" s="18" t="s">
+      <c r="A36" s="17"/>
+      <c r="B36" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="C36" s="8" t="str">
+      <c r="C36" s="23" t="str">
         <f t="shared" si="0"/>
         <v>3148, 5%</v>
       </c>
-      <c r="D36" s="8" t="str">
+      <c r="D36" s="23" t="str">
         <f t="shared" si="1"/>
         <v>418, 8%</v>
       </c>
-      <c r="E36" s="8" t="str">
+      <c r="E36" s="23" t="str">
         <f t="shared" si="2"/>
         <v>2730, 5%</v>
       </c>
-      <c r="F36" s="23"/>
+      <c r="F36" s="25"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="9">
+      <c r="H36" s="8">
         <v>3148</v>
       </c>
-      <c r="I36" s="10">
+      <c r="I36" s="9">
         <f t="shared" si="3"/>
         <v>5.4153549741101994E-2</v>
       </c>
-      <c r="J36" s="9">
+      <c r="J36" s="8">
         <v>418</v>
       </c>
-      <c r="K36" s="10">
+      <c r="K36" s="9">
         <f t="shared" si="4"/>
         <v>7.823320232079356E-2</v>
       </c>
-      <c r="L36" s="9">
+      <c r="L36" s="8">
         <v>2730</v>
       </c>
-      <c r="M36" s="10">
+      <c r="M36" s="9">
         <f t="shared" si="5"/>
         <v>5.1716299158899748E-2</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="18"/>
-      <c r="B37" s="18" t="s">
+      <c r="A37" s="17"/>
+      <c r="B37" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="C37" s="8" t="str">
+      <c r="C37" s="23" t="str">
         <f t="shared" si="0"/>
         <v>4774, 8%</v>
       </c>
-      <c r="D37" s="8" t="str">
+      <c r="D37" s="23" t="str">
         <f t="shared" si="1"/>
         <v>509, 10%</v>
       </c>
-      <c r="E37" s="8" t="str">
+      <c r="E37" s="23" t="str">
         <f t="shared" si="2"/>
         <v>4265, 8%</v>
       </c>
-      <c r="F37" s="23"/>
+      <c r="F37" s="25"/>
       <c r="G37" s="7"/>
-      <c r="H37" s="9">
+      <c r="H37" s="8">
         <v>4774</v>
       </c>
-      <c r="I37" s="10">
+      <c r="I37" s="9">
         <f t="shared" si="3"/>
         <v>8.2124855928850354E-2</v>
       </c>
-      <c r="J37" s="9">
+      <c r="J37" s="8">
         <v>509</v>
       </c>
-      <c r="K37" s="10">
+      <c r="K37" s="9">
         <f t="shared" si="4"/>
         <v>9.5264832491109869E-2</v>
       </c>
-      <c r="L37" s="9">
+      <c r="L37" s="8">
         <v>4265</v>
       </c>
-      <c r="M37" s="10">
+      <c r="M37" s="9">
         <f t="shared" si="5"/>
         <v>8.0794877623702355E-2</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A38" s="18"/>
-      <c r="B38" s="18" t="s">
+      <c r="A38" s="17"/>
+      <c r="B38" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C38" s="8" t="str">
+      <c r="C38" s="23" t="str">
         <f t="shared" si="0"/>
         <v>6491, 11%</v>
       </c>
-      <c r="D38" s="8" t="str">
+      <c r="D38" s="23" t="str">
         <f t="shared" si="1"/>
         <v>609, 11%</v>
       </c>
-      <c r="E38" s="8" t="str">
+      <c r="E38" s="23" t="str">
         <f t="shared" si="2"/>
         <v>5882, 11%</v>
       </c>
-      <c r="F38" s="23"/>
+      <c r="F38" s="25"/>
       <c r="G38" s="7"/>
-      <c r="H38" s="9">
+      <c r="H38" s="8">
         <v>6491</v>
       </c>
-      <c r="I38" s="10">
+      <c r="I38" s="9">
         <f t="shared" si="3"/>
         <v>0.1116615919216941</v>
       </c>
-      <c r="J38" s="9">
+      <c r="J38" s="8">
         <v>609</v>
       </c>
-      <c r="K38" s="10">
+      <c r="K38" s="9">
         <f t="shared" si="4"/>
         <v>0.11398090960134756</v>
       </c>
-      <c r="L38" s="9">
+      <c r="L38" s="8">
         <v>5882</v>
       </c>
-      <c r="M38" s="10">
+      <c r="M38" s="9">
         <f t="shared" si="5"/>
         <v>0.11142683943320451</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A39" s="18"/>
-      <c r="B39" s="18" t="s">
+      <c r="A39" s="17"/>
+      <c r="B39" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="C39" s="8" t="str">
+      <c r="C39" s="23" t="str">
         <f t="shared" si="0"/>
         <v>9305, 16%</v>
       </c>
-      <c r="D39" s="8" t="str">
+      <c r="D39" s="23" t="str">
         <f t="shared" si="1"/>
         <v>765, 14%</v>
       </c>
-      <c r="E39" s="8" t="str">
+      <c r="E39" s="23" t="str">
         <f t="shared" si="2"/>
         <v>8540, 16%</v>
       </c>
-      <c r="F39" s="23"/>
+      <c r="F39" s="25"/>
       <c r="G39" s="7"/>
-      <c r="H39" s="9">
+      <c r="H39" s="8">
         <v>9305</v>
       </c>
-      <c r="I39" s="10">
+      <c r="I39" s="9">
         <f t="shared" si="3"/>
         <v>0.1600694982023361</v>
       </c>
-      <c r="J39" s="9">
+      <c r="J39" s="8">
         <v>765</v>
       </c>
-      <c r="K39" s="10">
+      <c r="K39" s="9">
         <f t="shared" si="4"/>
         <v>0.14317798989331837</v>
       </c>
-      <c r="L39" s="9">
+      <c r="L39" s="8">
         <v>8540</v>
       </c>
-      <c r="M39" s="10">
+      <c r="M39" s="9">
         <f t="shared" si="5"/>
         <v>0.16177919224066076</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40" s="18"/>
-      <c r="B40" s="18" t="s">
+      <c r="A40" s="17"/>
+      <c r="B40" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="C40" s="8" t="str">
+      <c r="C40" s="23" t="str">
         <f t="shared" si="0"/>
         <v>9636, 17%</v>
       </c>
-      <c r="D40" s="8" t="str">
+      <c r="D40" s="23" t="str">
         <f t="shared" si="1"/>
         <v>825, 15%</v>
       </c>
-      <c r="E40" s="8" t="str">
+      <c r="E40" s="23" t="str">
         <f t="shared" si="2"/>
         <v>8811, 17%</v>
       </c>
-      <c r="F40" s="23"/>
+      <c r="F40" s="25"/>
       <c r="G40" s="7"/>
-      <c r="H40" s="9">
+      <c r="H40" s="8">
         <v>9636</v>
       </c>
-      <c r="I40" s="10">
+      <c r="I40" s="9">
         <f t="shared" si="3"/>
         <v>0.16576353408680394</v>
       </c>
-      <c r="J40" s="9">
+      <c r="J40" s="8">
         <v>825</v>
       </c>
-      <c r="K40" s="10">
+      <c r="K40" s="9">
         <f t="shared" si="4"/>
         <v>0.15440763615946099</v>
       </c>
-      <c r="L40" s="9">
+      <c r="L40" s="8">
         <v>8811</v>
       </c>
-      <c r="M40" s="10">
+      <c r="M40" s="9">
         <f t="shared" si="5"/>
         <v>0.16691293475789953</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" s="18"/>
-      <c r="B41" s="18" t="s">
+      <c r="A41" s="17"/>
+      <c r="B41" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="C41" s="8" t="str">
+      <c r="C41" s="23" t="str">
         <f t="shared" si="0"/>
         <v>15230, 26%</v>
       </c>
-      <c r="D41" s="8" t="str">
+      <c r="D41" s="23" t="str">
         <f t="shared" si="1"/>
         <v>1167, 22%</v>
       </c>
-      <c r="E41" s="8" t="str">
+      <c r="E41" s="23" t="str">
         <f t="shared" si="2"/>
         <v>14063, 27%</v>
       </c>
-      <c r="F41" s="23"/>
+      <c r="F41" s="25"/>
       <c r="G41" s="7"/>
-      <c r="H41" s="9">
+      <c r="H41" s="8">
         <v>15230</v>
       </c>
-      <c r="I41" s="10">
+      <c r="I41" s="9">
         <f t="shared" si="3"/>
         <v>0.26199446078684352</v>
       </c>
-      <c r="J41" s="9">
+      <c r="J41" s="8">
         <v>1167</v>
       </c>
-      <c r="K41" s="10">
+      <c r="K41" s="9">
         <f t="shared" si="4"/>
         <v>0.2184166198764739</v>
       </c>
-      <c r="L41" s="9">
+      <c r="L41" s="8">
         <v>14063</v>
       </c>
-      <c r="M41" s="10">
+      <c r="M41" s="9">
         <f t="shared" si="5"/>
         <v>0.26640524361597334</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42" s="18"/>
-      <c r="B42" s="18" t="s">
+      <c r="A42" s="17"/>
+      <c r="B42" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C42" s="8" t="str">
+      <c r="C42" s="23" t="str">
         <f t="shared" si="0"/>
         <v>6271, 11%</v>
       </c>
-      <c r="D42" s="8" t="str">
+      <c r="D42" s="23" t="str">
         <f t="shared" si="1"/>
         <v>558, 10%</v>
       </c>
-      <c r="E42" s="8" t="str">
+      <c r="E42" s="23" t="str">
         <f t="shared" si="2"/>
         <v>5713, 11%</v>
       </c>
-      <c r="F42" s="24"/>
+      <c r="F42" s="26"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="9">
+      <c r="H42" s="8">
         <v>6271</v>
       </c>
-      <c r="I42" s="10">
+      <c r="I42" s="9">
         <f t="shared" si="3"/>
         <v>0.10787703634893603</v>
       </c>
-      <c r="J42" s="9">
+      <c r="J42" s="8">
         <v>558</v>
       </c>
-      <c r="K42" s="10">
+      <c r="K42" s="9">
         <f t="shared" si="4"/>
         <v>0.10443571027512634</v>
       </c>
-      <c r="L42" s="9">
+      <c r="L42" s="8">
         <v>5713</v>
       </c>
-      <c r="M42" s="10">
+      <c r="M42" s="9">
         <f t="shared" si="5"/>
         <v>0.10822535424717739</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A43" s="18" t="s">
+      <c r="A43" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B43" s="18" t="s">
+      <c r="B43" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C43" s="8" t="str">
+      <c r="C43" s="23" t="str">
         <f t="shared" si="0"/>
         <v>478, 1%</v>
       </c>
-      <c r="D43" s="8" t="str">
+      <c r="D43" s="23" t="str">
         <f t="shared" si="1"/>
         <v>61, 1%</v>
       </c>
-      <c r="E43" s="8" t="str">
+      <c r="E43" s="23" t="str">
         <f t="shared" si="2"/>
         <v>417, 1%</v>
       </c>
-      <c r="F43" s="22" t="s">
+      <c r="F43" s="24" t="s">
         <v>79</v>
       </c>
       <c r="G43" s="7"/>
-      <c r="H43" s="9">
+      <c r="H43" s="8">
         <v>478</v>
       </c>
-      <c r="I43" s="10">
+      <c r="I43" s="9">
         <f t="shared" si="3"/>
         <v>8.2228071080834662E-3</v>
       </c>
-      <c r="J43" s="9">
+      <c r="J43" s="8">
         <v>61</v>
       </c>
-      <c r="K43" s="10">
+      <c r="K43" s="9">
         <f t="shared" si="4"/>
         <v>1.1416807037244993E-2</v>
       </c>
-      <c r="L43" s="9">
+      <c r="L43" s="8">
         <v>417</v>
       </c>
-      <c r="M43" s="10">
+      <c r="M43" s="9">
         <f t="shared" si="5"/>
         <v>7.899522618776994E-3</v>
       </c>
     </row>
     <row r="44" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A44" s="18"/>
-      <c r="B44" s="18" t="s">
+      <c r="A44" s="17"/>
+      <c r="B44" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C44" s="8" t="str">
+      <c r="C44" s="23" t="str">
         <f t="shared" si="0"/>
         <v>14340, 25%</v>
       </c>
-      <c r="D44" s="8" t="str">
+      <c r="D44" s="23" t="str">
         <f t="shared" si="1"/>
         <v>1171, 22%</v>
       </c>
-      <c r="E44" s="8" t="str">
+      <c r="E44" s="23" t="str">
         <f t="shared" si="2"/>
         <v>13169, 25%</v>
       </c>
-      <c r="F44" s="23"/>
+      <c r="F44" s="25"/>
       <c r="G44" s="7"/>
-      <c r="H44" s="9">
+      <c r="H44" s="8">
         <v>14340</v>
       </c>
-      <c r="I44" s="10">
+      <c r="I44" s="9">
         <f t="shared" si="3"/>
         <v>0.246684213242504</v>
       </c>
-      <c r="J44" s="9">
+      <c r="J44" s="8">
         <v>1171</v>
       </c>
-      <c r="K44" s="10">
+      <c r="K44" s="9">
         <f t="shared" si="4"/>
         <v>0.2191652629608834</v>
       </c>
-      <c r="L44" s="9">
+      <c r="L44" s="8">
         <v>13169</v>
       </c>
-      <c r="M44" s="10">
+      <c r="M44" s="9">
         <f t="shared" si="5"/>
         <v>0.24946957641888309</v>
       </c>
     </row>
     <row r="45" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A45" s="18"/>
-      <c r="B45" s="18" t="s">
+      <c r="A45" s="17"/>
+      <c r="B45" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C45" s="8" t="str">
+      <c r="C45" s="23" t="str">
         <f t="shared" si="0"/>
         <v>25572, 44%</v>
       </c>
-      <c r="D45" s="8" t="str">
+      <c r="D45" s="23" t="str">
         <f t="shared" si="1"/>
         <v>2098, 39%</v>
       </c>
-      <c r="E45" s="8" t="str">
+      <c r="E45" s="23" t="str">
         <f t="shared" si="2"/>
         <v>23474, 44%</v>
       </c>
-      <c r="F45" s="23"/>
+      <c r="F45" s="25"/>
       <c r="G45" s="7"/>
-      <c r="H45" s="9">
+      <c r="H45" s="8">
         <v>25572</v>
       </c>
-      <c r="I45" s="10">
+      <c r="I45" s="9">
         <f t="shared" si="3"/>
         <v>0.43990297775713477</v>
       </c>
-      <c r="J45" s="9">
+      <c r="J45" s="8">
         <v>2098</v>
       </c>
-      <c r="K45" s="10">
+      <c r="K45" s="9">
         <f t="shared" si="4"/>
         <v>0.3926632977727868</v>
       </c>
-      <c r="L45" s="9">
+      <c r="L45" s="8">
         <v>23474</v>
       </c>
-      <c r="M45" s="10">
+      <c r="M45" s="9">
         <f t="shared" si="5"/>
         <v>0.44468439796923542</v>
       </c>
     </row>
     <row r="46" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A46" s="18"/>
-      <c r="B46" s="18" t="s">
+      <c r="A46" s="17"/>
+      <c r="B46" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C46" s="8" t="str">
+      <c r="C46" s="23" t="str">
         <f t="shared" si="0"/>
         <v>16871, 29%</v>
       </c>
-      <c r="D46" s="8" t="str">
+      <c r="D46" s="23" t="str">
         <f t="shared" si="1"/>
         <v>1909, 36%</v>
       </c>
-      <c r="E46" s="8" t="str">
+      <c r="E46" s="23" t="str">
         <f t="shared" si="2"/>
         <v>14962, 28%</v>
       </c>
-      <c r="F46" s="23"/>
+      <c r="F46" s="25"/>
       <c r="G46" s="7"/>
-      <c r="H46" s="9">
+      <c r="H46" s="8">
         <v>16871</v>
       </c>
-      <c r="I46" s="10">
+      <c r="I46" s="9">
         <f t="shared" si="3"/>
         <v>0.29022380485455262</v>
       </c>
-      <c r="J46" s="9">
+      <c r="J46" s="8">
         <v>1909</v>
       </c>
-      <c r="K46" s="10">
+      <c r="K46" s="9">
         <f t="shared" si="4"/>
         <v>0.35728991203443761</v>
       </c>
-      <c r="L46" s="9">
+      <c r="L46" s="8">
         <v>14962</v>
       </c>
-      <c r="M46" s="10">
+      <c r="M46" s="9">
         <f t="shared" si="5"/>
         <v>0.28343562930969157</v>
       </c>
     </row>
     <row r="47" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A47" s="18"/>
-      <c r="B47" s="18" t="s">
+      <c r="A47" s="17"/>
+      <c r="B47" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C47" s="8" t="str">
+      <c r="C47" s="23" t="str">
         <f t="shared" si="0"/>
         <v>870, 1%</v>
       </c>
-      <c r="D47" s="8" t="str">
+      <c r="D47" s="23" t="str">
         <f t="shared" si="1"/>
         <v>104, 2%</v>
       </c>
-      <c r="E47" s="8" t="str">
+      <c r="E47" s="23" t="str">
         <f t="shared" si="2"/>
         <v>766, 1%</v>
       </c>
-      <c r="F47" s="24"/>
+      <c r="F47" s="26"/>
       <c r="G47" s="7"/>
-      <c r="H47" s="9">
+      <c r="H47" s="8">
         <v>870</v>
       </c>
-      <c r="I47" s="10">
+      <c r="I47" s="9">
         <f t="shared" si="3"/>
         <v>1.4966197037725138E-2</v>
       </c>
-      <c r="J47" s="9">
+      <c r="J47" s="8">
         <v>104</v>
       </c>
-      <c r="K47" s="10">
+      <c r="K47" s="9">
         <f t="shared" si="4"/>
         <v>1.9464720194647202E-2</v>
       </c>
-      <c r="L47" s="9">
+      <c r="L47" s="8">
         <v>766</v>
       </c>
-      <c r="M47" s="10">
+      <c r="M47" s="9">
         <f t="shared" si="5"/>
         <v>1.4510873683412896E-2</v>
       </c>
     </row>
     <row r="48" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A48" s="18" t="s">
+      <c r="A48" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B48" s="18" t="s">
+      <c r="B48" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C48" s="8" t="str">
+      <c r="C48" s="23" t="str">
         <f t="shared" si="0"/>
         <v>8571, 15%</v>
       </c>
-      <c r="D48" s="8" t="str">
+      <c r="D48" s="23" t="str">
         <f t="shared" si="1"/>
         <v>931, 17%</v>
       </c>
-      <c r="E48" s="8" t="str">
+      <c r="E48" s="23" t="str">
         <f t="shared" si="2"/>
         <v>7640, 14%</v>
       </c>
-      <c r="F48" s="22" t="s">
+      <c r="F48" s="24" t="s">
         <v>79</v>
       </c>
       <c r="G48" s="7"/>
-      <c r="H48" s="9">
+      <c r="H48" s="8">
         <v>8571</v>
       </c>
-      <c r="I48" s="10">
+      <c r="I48" s="9">
         <f t="shared" si="3"/>
         <v>0.14744284460958867</v>
       </c>
-      <c r="J48" s="9">
+      <c r="J48" s="8">
         <v>931</v>
       </c>
-      <c r="K48" s="10">
+      <c r="K48" s="9">
         <f t="shared" si="4"/>
         <v>0.17424667789631293</v>
       </c>
-      <c r="L48" s="9">
+      <c r="L48" s="8">
         <v>7640</v>
       </c>
-      <c r="M48" s="10">
+      <c r="M48" s="9">
         <f t="shared" si="5"/>
         <v>0.14472986284761688</v>
       </c>
     </row>
     <row r="49" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A49" s="18"/>
-      <c r="B49" s="18" t="s">
+      <c r="A49" s="17"/>
+      <c r="B49" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C49" s="8" t="str">
+      <c r="C49" s="23" t="str">
         <f t="shared" si="0"/>
         <v>26639, 46%</v>
       </c>
-      <c r="D49" s="8" t="str">
+      <c r="D49" s="23" t="str">
         <f t="shared" si="1"/>
         <v>4389, 82%</v>
       </c>
-      <c r="E49" s="8" t="str">
+      <c r="E49" s="23" t="str">
         <f t="shared" si="2"/>
         <v>44872, 85%</v>
       </c>
-      <c r="F49" s="23"/>
+      <c r="F49" s="25"/>
       <c r="G49" s="7"/>
-      <c r="H49" s="9">
+      <c r="H49" s="8">
         <v>26639</v>
       </c>
-      <c r="I49" s="10">
+      <c r="I49" s="9">
         <f t="shared" si="3"/>
         <v>0.45825807228501142</v>
       </c>
-      <c r="J49" s="9">
+      <c r="J49" s="8">
         <v>4389</v>
       </c>
-      <c r="K49" s="10">
+      <c r="K49" s="9">
         <f t="shared" si="4"/>
         <v>0.82144862436833244</v>
       </c>
-      <c r="L49" s="9">
+      <c r="L49" s="8">
         <v>44872</v>
       </c>
-      <c r="M49" s="10">
+      <c r="M49" s="9">
         <f t="shared" si="5"/>
         <v>0.85004167613851633</v>
       </c>
     </row>
     <row r="50" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A50" s="18"/>
-      <c r="B50" s="18" t="s">
+      <c r="A50" s="17"/>
+      <c r="B50" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C50" s="8" t="str">
+      <c r="C50" s="23" t="str">
         <f t="shared" si="0"/>
         <v>22921, 39%</v>
       </c>
-      <c r="D50" s="8" t="str">
+      <c r="D50" s="23" t="str">
         <f t="shared" si="1"/>
         <v>23, 0%</v>
       </c>
-      <c r="E50" s="8" t="str">
+      <c r="E50" s="23" t="str">
         <f t="shared" si="2"/>
         <v>276, 1%</v>
       </c>
-      <c r="F50" s="24"/>
+      <c r="F50" s="26"/>
       <c r="G50" s="7"/>
-      <c r="H50" s="9">
+      <c r="H50" s="8">
         <v>22921</v>
       </c>
-      <c r="I50" s="10">
+      <c r="I50" s="9">
         <f t="shared" si="3"/>
         <v>0.39429908310539985</v>
       </c>
-      <c r="J50" s="9">
+      <c r="J50" s="8">
         <v>23</v>
       </c>
-      <c r="K50" s="10">
+      <c r="K50" s="9">
         <f t="shared" si="4"/>
         <v>4.3046977353546701E-3</v>
       </c>
-      <c r="L50" s="9">
+      <c r="L50" s="8">
         <v>276</v>
       </c>
-      <c r="M50" s="10">
+      <c r="M50" s="9">
         <f t="shared" si="5"/>
         <v>5.2284610138667881E-3</v>
       </c>
     </row>
     <row r="51" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A51" s="18" t="s">
+      <c r="A51" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B51" s="18" t="s">
+      <c r="B51" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C51" s="8" t="str">
+      <c r="C51" s="23" t="str">
         <f t="shared" si="0"/>
         <v>8571, 15%</v>
       </c>
-      <c r="D51" s="8" t="str">
+      <c r="D51" s="23" t="str">
         <f t="shared" si="1"/>
         <v>3759, 70%</v>
       </c>
-      <c r="E51" s="8" t="str">
+      <c r="E51" s="23" t="str">
         <f t="shared" si="2"/>
         <v>40598, 77%</v>
       </c>
-      <c r="F51" s="22" t="s">
+      <c r="F51" s="24" t="s">
         <v>79</v>
       </c>
       <c r="G51" s="7"/>
-      <c r="H51" s="9">
+      <c r="H51" s="8">
         <v>8571</v>
       </c>
-      <c r="I51" s="10">
+      <c r="I51" s="9">
         <f t="shared" si="3"/>
         <v>0.14744284460958867</v>
       </c>
-      <c r="J51" s="9">
+      <c r="J51" s="8">
         <v>3759</v>
       </c>
-      <c r="K51" s="10">
+      <c r="K51" s="9">
         <f t="shared" si="4"/>
         <v>0.70353733857383494</v>
       </c>
-      <c r="L51" s="9">
+      <c r="L51" s="8">
         <v>40598</v>
       </c>
-      <c r="M51" s="10">
+      <c r="M51" s="9">
         <f t="shared" si="5"/>
         <v>0.76907630522088355</v>
       </c>
     </row>
     <row r="52" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A52" s="18"/>
-      <c r="B52" s="18" t="s">
+      <c r="A52" s="17"/>
+      <c r="B52" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C52" s="8" t="str">
+      <c r="C52" s="23" t="str">
         <f t="shared" si="0"/>
         <v>49261, 85%</v>
       </c>
-      <c r="D52" s="8" t="str">
+      <c r="D52" s="23" t="str">
         <f t="shared" si="1"/>
         <v>1572, 29%</v>
       </c>
-      <c r="E52" s="8" t="str">
+      <c r="E52" s="23" t="str">
         <f t="shared" si="2"/>
         <v>12069, 23%</v>
       </c>
-      <c r="F52" s="23"/>
+      <c r="F52" s="25"/>
       <c r="G52" s="7"/>
-      <c r="H52" s="9">
+      <c r="H52" s="8">
         <v>49261</v>
       </c>
-      <c r="I52" s="10">
+      <c r="I52" s="9">
         <f t="shared" si="3"/>
         <v>0.84741360031652646</v>
       </c>
-      <c r="J52" s="9">
+      <c r="J52" s="8">
         <v>1572</v>
       </c>
-      <c r="K52" s="10">
+      <c r="K52" s="9">
         <f t="shared" si="4"/>
         <v>0.29421673217293653</v>
       </c>
-      <c r="L52" s="9">
+      <c r="L52" s="8">
         <v>12069</v>
       </c>
-      <c r="M52" s="10">
+      <c r="M52" s="9">
         <f t="shared" si="5"/>
         <v>0.22863150716071834</v>
       </c>
     </row>
     <row r="53" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A53" s="18"/>
-      <c r="B53" s="18" t="s">
+      <c r="A53" s="17"/>
+      <c r="B53" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C53" s="8" t="str">
+      <c r="C53" s="23" t="str">
         <f t="shared" si="0"/>
         <v>299, 1%</v>
       </c>
-      <c r="D53" s="8" t="str">
+      <c r="D53" s="23" t="str">
         <f t="shared" si="1"/>
         <v>12, 0%</v>
       </c>
-      <c r="E53" s="8" t="str">
+      <c r="E53" s="23" t="str">
         <f t="shared" si="2"/>
         <v>121, 0%</v>
       </c>
-      <c r="F53" s="24"/>
+      <c r="F53" s="26"/>
       <c r="G53" s="7"/>
-      <c r="H53" s="9">
+      <c r="H53" s="8">
         <v>299</v>
       </c>
-      <c r="I53" s="10">
+      <c r="I53" s="9">
         <f t="shared" si="3"/>
         <v>5.1435550738848463E-3</v>
       </c>
-      <c r="J53" s="9">
+      <c r="J53" s="8">
         <v>12</v>
       </c>
-      <c r="K53" s="10">
+      <c r="K53" s="9">
         <f t="shared" si="4"/>
         <v>2.2459292532285235E-3</v>
       </c>
-      <c r="L53" s="9">
+      <c r="L53" s="8">
         <v>121</v>
       </c>
-      <c r="M53" s="10">
+      <c r="M53" s="9">
         <f t="shared" si="5"/>
         <v>2.2921876183981207E-3</v>
       </c>
     </row>
     <row r="54" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A54" s="18" t="s">
+      <c r="A54" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="B54" s="18" t="s">
+      <c r="B54" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="C54" s="8" t="str">
+      <c r="C54" s="23" t="str">
         <f t="shared" si="0"/>
         <v>55795, 96%</v>
       </c>
-      <c r="D54" s="8" t="str">
+      <c r="D54" s="23" t="str">
         <f t="shared" si="1"/>
         <v>5095, 95%</v>
       </c>
-      <c r="E54" s="8" t="str">
+      <c r="E54" s="23" t="str">
         <f t="shared" si="2"/>
         <v>50700, 96%</v>
       </c>
-      <c r="F54" s="22">
+      <c r="F54" s="24">
         <v>4.1759999999999999E-2</v>
       </c>
       <c r="G54" s="7"/>
-      <c r="H54" s="9">
+      <c r="H54" s="8">
         <v>55795</v>
       </c>
-      <c r="I54" s="10">
+      <c r="I54" s="9">
         <f t="shared" si="3"/>
         <v>0.95981490082744148</v>
       </c>
-      <c r="J54" s="9">
+      <c r="J54" s="8">
         <v>5095</v>
       </c>
-      <c r="K54" s="10">
+      <c r="K54" s="9">
         <f t="shared" si="4"/>
         <v>0.95358412876661047</v>
       </c>
-      <c r="L54" s="9">
+      <c r="L54" s="8">
         <v>50700</v>
       </c>
-      <c r="M54" s="10">
+      <c r="M54" s="9">
         <f t="shared" si="5"/>
         <v>0.96044555580813817</v>
       </c>
     </row>
     <row r="55" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A55" s="18"/>
-      <c r="B55" s="18" t="s">
+      <c r="A55" s="17"/>
+      <c r="B55" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="C55" s="8" t="str">
+      <c r="C55" s="23" t="str">
         <f t="shared" si="0"/>
         <v>2203, 4%</v>
       </c>
-      <c r="D55" s="8" t="str">
+      <c r="D55" s="23" t="str">
         <f t="shared" si="1"/>
         <v>236, 4%</v>
       </c>
-      <c r="E55" s="8" t="str">
+      <c r="E55" s="23" t="str">
         <f t="shared" si="2"/>
         <v>1967, 4%</v>
       </c>
-      <c r="F55" s="23"/>
+      <c r="F55" s="25"/>
       <c r="G55" s="7"/>
-      <c r="H55" s="9">
+      <c r="H55" s="8">
         <v>2203</v>
       </c>
-      <c r="I55" s="10">
+      <c r="I55" s="9">
         <f t="shared" si="3"/>
         <v>3.7897163303572963E-2</v>
       </c>
-      <c r="J55" s="9">
+      <c r="J55" s="8">
         <v>236</v>
       </c>
-      <c r="K55" s="10">
+      <c r="K55" s="9">
         <f t="shared" si="4"/>
         <v>4.4169941980160957E-2</v>
       </c>
-      <c r="L55" s="9">
+      <c r="L55" s="8">
         <v>1967</v>
       </c>
-      <c r="M55" s="10">
+      <c r="M55" s="9">
         <f t="shared" si="5"/>
         <v>3.7262256573463666E-2</v>
       </c>
     </row>
     <row r="56" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A56" s="18"/>
-      <c r="B56" s="18" t="s">
+      <c r="A56" s="17"/>
+      <c r="B56" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C56" s="8" t="str">
+      <c r="C56" s="23" t="str">
         <f t="shared" si="0"/>
         <v>133, 0%</v>
       </c>
-      <c r="D56" s="8" t="str">
+      <c r="D56" s="23" t="str">
         <f t="shared" si="1"/>
         <v>12, 0%</v>
       </c>
-      <c r="E56" s="8" t="str">
+      <c r="E56" s="23" t="str">
         <f t="shared" si="2"/>
         <v>121, 0%</v>
       </c>
-      <c r="F56" s="24"/>
+      <c r="F56" s="26"/>
       <c r="G56" s="7"/>
-      <c r="H56" s="9">
+      <c r="H56" s="8">
         <v>133</v>
       </c>
-      <c r="I56" s="10">
+      <c r="I56" s="9">
         <f t="shared" si="3"/>
         <v>2.2879358689855672E-3</v>
       </c>
-      <c r="J56" s="9">
+      <c r="J56" s="8">
         <v>12</v>
       </c>
-      <c r="K56" s="10">
+      <c r="K56" s="9">
         <f t="shared" si="4"/>
         <v>2.2459292532285235E-3</v>
       </c>
-      <c r="L56" s="9">
+      <c r="L56" s="8">
         <v>121</v>
       </c>
-      <c r="M56" s="10">
+      <c r="M56" s="9">
         <f t="shared" si="5"/>
         <v>2.2921876183981207E-3</v>
       </c>
     </row>
     <row r="57" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A57" s="18" t="s">
+      <c r="A57" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="B57" s="18" t="s">
+      <c r="B57" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C57" s="8" t="str">
+      <c r="C57" s="23" t="str">
         <f t="shared" si="0"/>
         <v>9016, 16%</v>
       </c>
-      <c r="D57" s="8" t="str">
+      <c r="D57" s="23" t="str">
         <f t="shared" si="1"/>
         <v>465, 9%</v>
       </c>
-      <c r="E57" s="8" t="str">
+      <c r="E57" s="23" t="str">
         <f t="shared" si="2"/>
         <v>8551, 16%</v>
       </c>
-      <c r="F57" s="22" t="s">
+      <c r="F57" s="24" t="s">
         <v>79</v>
       </c>
       <c r="G57" s="7"/>
-      <c r="H57" s="9">
+      <c r="H57" s="8">
         <v>9016</v>
       </c>
-      <c r="I57" s="10">
+      <c r="I57" s="9">
         <f t="shared" si="3"/>
         <v>0.15509796838175843</v>
       </c>
-      <c r="J57" s="9">
+      <c r="J57" s="8">
         <v>465</v>
       </c>
-      <c r="K57" s="10">
+      <c r="K57" s="9">
         <f t="shared" si="4"/>
         <v>8.7029758562605281E-2</v>
       </c>
-      <c r="L57" s="9">
+      <c r="L57" s="8">
         <v>8551</v>
       </c>
-      <c r="M57" s="10">
+      <c r="M57" s="9">
         <f t="shared" si="5"/>
         <v>0.1619875729332424</v>
       </c>
     </row>
     <row r="58" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A58" s="18"/>
-      <c r="B58" s="18" t="s">
+      <c r="A58" s="17"/>
+      <c r="B58" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C58" s="8" t="str">
+      <c r="C58" s="23" t="str">
         <f t="shared" si="0"/>
         <v>18111, 31%</v>
       </c>
-      <c r="D58" s="8" t="str">
+      <c r="D58" s="23" t="str">
         <f t="shared" si="1"/>
         <v>1253, 23%</v>
       </c>
-      <c r="E58" s="8" t="str">
+      <c r="E58" s="23" t="str">
         <f t="shared" si="2"/>
         <v>16858, 32%</v>
       </c>
-      <c r="F58" s="23"/>
+      <c r="F58" s="25"/>
       <c r="G58" s="7"/>
-      <c r="H58" s="9">
+      <c r="H58" s="8">
         <v>18111</v>
       </c>
-      <c r="I58" s="10">
+      <c r="I58" s="9">
         <f t="shared" si="3"/>
         <v>0.31155493626464364</v>
       </c>
-      <c r="J58" s="9">
+      <c r="J58" s="8">
         <v>1253</v>
       </c>
-      <c r="K58" s="10">
+      <c r="K58" s="9">
         <f t="shared" si="4"/>
         <v>0.23451244619127831</v>
       </c>
-      <c r="L58" s="9">
+      <c r="L58" s="8">
         <v>16858</v>
       </c>
-      <c r="M58" s="10">
+      <c r="M58" s="9">
         <f t="shared" si="5"/>
         <v>0.31935288323103733</v>
       </c>
     </row>
     <row r="59" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A59" s="18"/>
-      <c r="B59" s="18" t="s">
+      <c r="A59" s="17"/>
+      <c r="B59" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C59" s="8" t="str">
+      <c r="C59" s="23" t="str">
         <f t="shared" si="0"/>
         <v>18797, 32%</v>
       </c>
-      <c r="D59" s="8" t="str">
+      <c r="D59" s="23" t="str">
         <f t="shared" si="1"/>
         <v>1741, 33%</v>
       </c>
-      <c r="E59" s="8" t="str">
+      <c r="E59" s="23" t="str">
         <f t="shared" si="2"/>
         <v>17056, 32%</v>
       </c>
-      <c r="F59" s="23"/>
+      <c r="F59" s="25"/>
       <c r="G59" s="7"/>
-      <c r="H59" s="9">
+      <c r="H59" s="8">
         <v>18797</v>
       </c>
-      <c r="I59" s="10">
+      <c r="I59" s="9">
         <f t="shared" si="3"/>
         <v>0.32335586864151655</v>
       </c>
-      <c r="J59" s="9">
+      <c r="J59" s="8">
         <v>1741</v>
       </c>
-      <c r="K59" s="10">
+      <c r="K59" s="9">
         <f t="shared" si="4"/>
         <v>0.32584690248923825</v>
       </c>
-      <c r="L59" s="9">
+      <c r="L59" s="8">
         <v>17056</v>
       </c>
-      <c r="M59" s="10">
+      <c r="M59" s="9">
         <f t="shared" si="5"/>
         <v>0.323103735697507</v>
       </c>
     </row>
     <row r="60" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A60" s="18"/>
-      <c r="B60" s="18" t="s">
+      <c r="A60" s="17"/>
+      <c r="B60" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C60" s="8" t="str">
+      <c r="C60" s="23" t="str">
         <f t="shared" si="0"/>
         <v>8436, 15%</v>
       </c>
-      <c r="D60" s="8" t="str">
+      <c r="D60" s="23" t="str">
         <f t="shared" si="1"/>
         <v>1187, 22%</v>
       </c>
-      <c r="E60" s="8" t="str">
+      <c r="E60" s="23" t="str">
         <f t="shared" si="2"/>
         <v>7249, 14%</v>
       </c>
-      <c r="F60" s="23"/>
+      <c r="F60" s="25"/>
       <c r="G60" s="7"/>
-      <c r="H60" s="9">
+      <c r="H60" s="8">
         <v>8436</v>
       </c>
-      <c r="I60" s="10">
+      <c r="I60" s="9">
         <f t="shared" si="3"/>
         <v>0.14512050368994167</v>
       </c>
-      <c r="J60" s="9">
+      <c r="J60" s="8">
         <v>1187</v>
       </c>
-      <c r="K60" s="10">
+      <c r="K60" s="9">
         <f t="shared" si="4"/>
         <v>0.22215983529852143</v>
       </c>
-      <c r="L60" s="9">
+      <c r="L60" s="8">
         <v>7249</v>
       </c>
-      <c r="M60" s="10">
+      <c r="M60" s="9">
         <f t="shared" si="5"/>
         <v>0.13732287641130561</v>
       </c>
     </row>
     <row r="61" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A61" s="18"/>
-      <c r="B61" s="18" t="s">
+      <c r="A61" s="17"/>
+      <c r="B61" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="C61" s="8" t="str">
+      <c r="C61" s="23" t="str">
         <f t="shared" si="0"/>
         <v>3569, 6%</v>
       </c>
-      <c r="D61" s="8" t="str">
+      <c r="D61" s="23" t="str">
         <f t="shared" si="1"/>
         <v>673, 13%</v>
       </c>
-      <c r="E61" s="8" t="str">
+      <c r="E61" s="23" t="str">
         <f t="shared" si="2"/>
         <v>2896, 5%</v>
       </c>
-      <c r="F61" s="23"/>
+      <c r="F61" s="25"/>
       <c r="G61" s="7"/>
-      <c r="H61" s="9">
+      <c r="H61" s="8">
         <v>3569</v>
       </c>
-      <c r="I61" s="10">
+      <c r="I61" s="9">
         <f t="shared" si="3"/>
         <v>6.1395812905334503E-2</v>
       </c>
-      <c r="J61" s="9">
+      <c r="J61" s="8">
         <v>673</v>
       </c>
-      <c r="K61" s="10">
+      <c r="K61" s="9">
         <f t="shared" si="4"/>
         <v>0.12595919895189969</v>
       </c>
-      <c r="L61" s="9">
+      <c r="L61" s="8">
         <v>2896</v>
       </c>
-      <c r="M61" s="10">
+      <c r="M61" s="9">
         <f t="shared" si="5"/>
         <v>5.4860953246950062E-2</v>
       </c>
     </row>
     <row r="62" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A62" s="18"/>
-      <c r="B62" s="18" t="s">
+      <c r="A62" s="17"/>
+      <c r="B62" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C62" s="8" t="str">
+      <c r="C62" s="23" t="str">
         <f t="shared" si="0"/>
         <v>202, 0%</v>
       </c>
-      <c r="D62" s="8" t="str">
+      <c r="D62" s="23" t="str">
         <f t="shared" si="1"/>
         <v>24, 0%</v>
       </c>
-      <c r="E62" s="8" t="str">
+      <c r="E62" s="23" t="str">
         <f t="shared" si="2"/>
         <v>178, 0%</v>
       </c>
-      <c r="F62" s="24"/>
+      <c r="F62" s="26"/>
       <c r="G62" s="7"/>
-      <c r="H62" s="9">
+      <c r="H62" s="8">
         <v>202</v>
       </c>
-      <c r="I62" s="10">
+      <c r="I62" s="9">
         <f t="shared" si="3"/>
         <v>3.474910116805147E-3</v>
       </c>
-      <c r="J62" s="9">
+      <c r="J62" s="8">
         <v>24</v>
       </c>
-      <c r="K62" s="10">
+      <c r="K62" s="9">
         <f t="shared" si="4"/>
         <v>4.4918585064570469E-3</v>
       </c>
-      <c r="L62" s="9">
+      <c r="L62" s="8">
         <v>178</v>
       </c>
-      <c r="M62" s="10">
+      <c r="M62" s="9">
         <f t="shared" si="5"/>
         <v>3.3719784799575662E-3</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="F25:F28"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="F7:F12"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="F18:F24"/>
     <mergeCell ref="F54:F56"/>
     <mergeCell ref="F57:F62"/>
     <mergeCell ref="F29:F33"/>
@@ -3514,13 +3542,6 @@
     <mergeCell ref="F43:F47"/>
     <mergeCell ref="F48:F50"/>
     <mergeCell ref="F51:F53"/>
-    <mergeCell ref="F25:F28"/>
-    <mergeCell ref="F4:F6"/>
-    <mergeCell ref="F7:F12"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="F18:F24"/>
-    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="72" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>